<commit_message>
Modified state names and descriptions per input from 3ric
</commit_message>
<xml_diff>
--- a/doc/systems/HackerboatArduinoStateTransitions.xlsx
+++ b/doc/systems/HackerboatArduinoStateTransitions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="46">
   <si>
     <t>Origin State</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Trigger Condition</t>
-  </si>
-  <si>
-    <t>Start</t>
   </si>
   <si>
     <t>internal</t>
@@ -152,37 +149,19 @@
     <t>Disarmed</t>
   </si>
   <si>
-    <t>All tests pass</t>
-  </si>
-  <si>
-    <t>Halt</t>
-  </si>
-  <si>
     <t xml:space="preserve">No heartbeat detected from the Beaglebone for 60 seconds. </t>
   </si>
   <si>
-    <t xml:space="preserve">If the failure was caused by no heartbeat and no other cause, presence of the heartbeat will cause it to recover. </t>
-  </si>
-  <si>
     <t>enable switch</t>
   </si>
   <si>
     <t>Enable switch is pressed and held for not less than 10 seconds.</t>
   </si>
   <si>
-    <t>Steering</t>
-  </si>
-  <si>
     <t>Low Battery</t>
   </si>
   <si>
-    <t>Panic</t>
-  </si>
-  <si>
     <t>stop switch</t>
-  </si>
-  <si>
-    <t>Stop switch is pressed and held for not less than 10 seconds.</t>
   </si>
   <si>
     <t>No heartbeat detected from the Beaglebone for 5 minutes.</t>
@@ -217,68 +196,61 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>V</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>battery</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &gt; 10V and Halt is last state</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>V</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>battery</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &gt; 10V and Steering is last state</t>
-    </r>
-  </si>
-  <si>
-    <t>Halt command received</t>
-  </si>
-  <si>
-    <t>Inhibited by activation of the Stop switch until the Enable switch has been off for not less than ten seconds. Also inhibited if Beaglebone is in Self-Test or Fault state.</t>
-  </si>
-  <si>
-    <t>Inhibited while Beaglebone is active in the Self-Test state or no valid state can be determined</t>
-  </si>
-  <si>
     <t>Inhibits</t>
+  </si>
+  <si>
+    <t>Armed</t>
+  </si>
+  <si>
+    <t>Armed command received</t>
+  </si>
+  <si>
+    <t>Vbattery &gt; 10V and Armed is last state</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Vbattery &gt; 10V and Active is last state</t>
+  </si>
+  <si>
+    <t>Active command received</t>
+  </si>
+  <si>
+    <t>Self Recovery</t>
+  </si>
+  <si>
+    <t>Beaglebone is in Self-Test or Fault state. No valid Beaglebone state.</t>
+  </si>
+  <si>
+    <t>All tests pass no other state is indicated in NVM</t>
+  </si>
+  <si>
+    <t>NVM</t>
+  </si>
+  <si>
+    <t>All tests pass and the last state in NVM is 'Active'</t>
+  </si>
+  <si>
+    <t>All tests pass and the last state in NVM is 'Armed'</t>
+  </si>
+  <si>
+    <t>All test pass except beaglebone heartbeat and the last in NVM is 'Active' or 'Armed'.</t>
+  </si>
+  <si>
+    <t>Beaglebone is in Self-Test.</t>
+  </si>
+  <si>
+    <t>No heartbeat detected from the Beaglebone for 60 seconds or Beaglebone is in Fault state.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the failure was caused by no heartbeat or Fault state and no other cause, presence of the heartbeat and a good Beaglebone state will cause it to recover. </t>
+  </si>
+  <si>
+    <t>Power Up</t>
+  </si>
+  <si>
+    <t>Stop switch is pressed and held for not less than 1 seconds.</t>
   </si>
 </sst>
 </file>
@@ -625,16 +597,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F25"/>
+  <dimension ref="A2:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="46.6640625" style="1" customWidth="1"/>
@@ -654,338 +626,389 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="E16" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
         <v>28</v>
       </c>
-      <c r="C21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added hardware test code Various modifications to 'as-built' condition Added TODO.md
</commit_message>
<xml_diff>
--- a/doc/systems/HackerboatArduinoStateTransitions.xlsx
+++ b/doc/systems/HackerboatArduinoStateTransitions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="47">
   <si>
     <t>Origin State</t>
   </si>
@@ -603,16 +603,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A2:F29"/>
+  <dimension ref="A2:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.21875" style="1" customWidth="1"/>
@@ -639,7 +638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -653,7 +652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -667,7 +666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -681,7 +680,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -695,7 +694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -709,7 +708,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -723,7 +722,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -740,7 +739,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -757,7 +756,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -774,7 +773,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -791,7 +790,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -805,7 +804,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -819,7 +818,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -833,7 +832,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -976,7 +975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -990,7 +989,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1004,7 +1003,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1018,7 +1017,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1032,15 +1031,18 @@
         <v>43</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:F29">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Active"/>
-        <filter val="Armed"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:F29"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
mapping Beaglebone message fields to Beaglebone states
</commit_message>
<xml_diff>
--- a/doc/systems/HackerboatArduinoStateTransitions.xlsx
+++ b/doc/systems/HackerboatArduinoStateTransitions.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BeagleBone Received Signals" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$F$29</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="76">
   <si>
     <t>Origin State</t>
   </si>
@@ -257,6 +258,93 @@
   </si>
   <si>
     <t>Disarm command received from the Beagelbone</t>
+  </si>
+  <si>
+    <t>BONE_POWERUP,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/**&lt; Initial starting state </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  BONE_SELFTEST,</t>
+  </si>
+  <si>
+    <t>/**&lt; Initial self-test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  BONE_DISARMED,</t>
+  </si>
+  <si>
+    <t>/**&lt; Disarmed wait state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  BONE_ARMED,</t>
+  </si>
+  <si>
+    <t>/**&lt; Beaglebone armed &amp; ready to navigate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  BONE_WAYPOINT,</t>
+  </si>
+  <si>
+    <t>/**&lt; Beaglebone navigating by waypoints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  BONE_STEERING,</t>
+  </si>
+  <si>
+    <t>/**&lt; Beaglebone manual steering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  BONE_NOSIGNAL,</t>
+  </si>
+  <si>
+    <t>/**&lt; Beaglbone has lost shore signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  BONE_FAULT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/**&lt; Beaglebone faulted </t>
+  </si>
+  <si>
+    <t>base mode (MAV_MODE)</t>
+  </si>
+  <si>
+    <t>system status (MAV_STATE)</t>
+  </si>
+  <si>
+    <t>Light pattern</t>
+  </si>
+  <si>
+    <t>MAV_MODE_PREFLIGHT</t>
+  </si>
+  <si>
+    <t>MAV_STATE_BOOT</t>
+  </si>
+  <si>
+    <t>MAV_STATE_STANDBY</t>
+  </si>
+  <si>
+    <t>MAV_MODE_MANUAL_DISARMED</t>
+  </si>
+  <si>
+    <t>MAV_MODE_MANUAL_ARMED</t>
+  </si>
+  <si>
+    <t>MAV_MODE_AUTO_ARMED</t>
+  </si>
+  <si>
+    <t>MAV_STATE_ACTIVE</t>
+  </si>
+  <si>
+    <t>MAV_STATE_EMERGENCY</t>
+  </si>
+  <si>
+    <t>MAV_STATE_CRITICAL</t>
+  </si>
+  <si>
+    <t>Any</t>
   </si>
 </sst>
 </file>
@@ -605,7 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -1046,4 +1134,167 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel decided to save these, not sure why
</commit_message>
<xml_diff>
--- a/doc/systems/HackerboatArduinoStateTransitions.xlsx
+++ b/doc/systems/HackerboatArduinoStateTransitions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -693,7 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -1140,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>